<commit_message>
Tested Date and Custom Converter
</commit_message>
<xml_diff>
--- a/src/test/resources/person-data.xlsx
+++ b/src/test/resources/person-data.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -33,6 +33,12 @@
   </si>
   <si>
     <t xml:space="preserve">Is Resident</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Birhdate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Account Value</t>
   </si>
   <si>
     <t xml:space="preserve">John</t>
@@ -87,8 +93,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -158,8 +165,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -180,10 +191,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+      <selection pane="topLeft" activeCell="J27" activeCellId="0" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -204,20 +215,32 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D2" s="0" t="n">
         <f aca="false">IF(1,TRUE())</f>
         <v>1</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>32874</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -225,29 +248,41 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D3" s="0" t="n">
         <f aca="false">IF(0,TRUE())</f>
         <v>0</v>
       </c>
+      <c r="E3" s="1" t="n">
+        <v>29221</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>2000</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D4" s="0" t="n">
         <f aca="false">IF(1,TRUE())</f>
         <v>1</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>27395</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>5000</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -255,14 +290,20 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D5" s="0" t="n">
         <f aca="false">IF(1,TRUE())</f>
         <v>1</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>31048</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>10000</v>
       </c>
     </row>
   </sheetData>
@@ -301,13 +342,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -318,10 +359,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -332,10 +373,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -346,10 +387,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -360,10 +401,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tested LocalDate and LocalDateTime
</commit_message>
<xml_diff>
--- a/src/test/resources/person-data.xlsx
+++ b/src/test/resources/person-data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Person" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -69,6 +69,12 @@
   </si>
   <si>
     <t xml:space="preserve">Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valid To</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check In</t>
   </si>
   <si>
     <t xml:space="preserve">Kraków Pawia 1</t>
@@ -93,9 +99,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
+    <numFmt numFmtId="166" formatCode="YYYY\-MM\-DD\ HH:MM"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -165,12 +172,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -193,8 +204,8 @@
   </sheetPr>
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J27" activeCellId="0" sqref="J27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -322,10 +333,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -334,7 +345,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.21"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="27.09"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -350,6 +363,12 @@
       <c r="D1" s="0" t="s">
         <v>15</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -359,10 +378,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>44196</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>40188.53125</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -373,10 +398,16 @@
         <v>1</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>45657</v>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>40189.40625</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -387,10 +418,16 @@
         <v>2</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>47848</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>40190.7814236111</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -401,10 +438,16 @@
         <v>3</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>43830</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>40191.8333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tested LocalTime and Float
</commit_message>
<xml_diff>
--- a/src/test/resources/person-data.xlsx
+++ b/src/test/resources/person-data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Person" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -39,6 +39,12 @@
   </si>
   <si>
     <t xml:space="preserve">Account Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Workday start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quality Factor</t>
   </si>
   <si>
     <t xml:space="preserve">John</t>
@@ -99,10 +105,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
-    <numFmt numFmtId="166" formatCode="YYYY\-MM\-DD\ HH:MM"/>
+    <numFmt numFmtId="166" formatCode="HH:MM:SS"/>
+    <numFmt numFmtId="167" formatCode="YYYY\-MM\-DD\ HH:MM"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -172,7 +179,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -182,6 +189,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -202,10 +213,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J12" activeCellId="0" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -232,16 +243,22 @@
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D2" s="0" t="n">
         <f aca="false">IF(1,TRUE())</f>
@@ -252,6 +269,12 @@
       </c>
       <c r="F2" s="0" t="n">
         <v>1000</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -259,10 +282,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D3" s="0" t="n">
         <f aca="false">IF(0,TRUE())</f>
@@ -274,16 +297,22 @@
       <c r="F3" s="0" t="n">
         <v>2000</v>
       </c>
+      <c r="G3" s="2" t="n">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D4" s="0" t="n">
         <f aca="false">IF(1,TRUE())</f>
@@ -294,6 +323,12 @@
       </c>
       <c r="F4" s="0" t="n">
         <v>5000</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>0.85</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -301,10 +336,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D5" s="0" t="n">
         <f aca="false">IF(1,TRUE())</f>
@@ -315,6 +350,12 @@
       </c>
       <c r="F5" s="0" t="n">
         <v>10000</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>0.3125</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>0.4</v>
       </c>
     </row>
   </sheetData>
@@ -335,7 +376,7 @@
   </sheetPr>
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -355,19 +396,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -378,15 +419,15 @@
         <v>1</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>44196</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="F2" s="3" t="n">
         <v>40188.53125</v>
       </c>
     </row>
@@ -398,15 +439,15 @@
         <v>1</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>45657</v>
       </c>
-      <c r="F3" s="2" t="n">
+      <c r="F3" s="3" t="n">
         <v>40189.40625</v>
       </c>
     </row>
@@ -418,15 +459,15 @@
         <v>2</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>47848</v>
       </c>
-      <c r="F4" s="2" t="n">
+      <c r="F4" s="3" t="n">
         <v>40190.7814236111</v>
       </c>
     </row>
@@ -438,15 +479,15 @@
         <v>3</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>43830</v>
       </c>
-      <c r="F5" s="2" t="n">
+      <c r="F5" s="3" t="n">
         <v>40191.8333333333</v>
       </c>
     </row>

</xml_diff>

<commit_message>
1. Fix defects:   - iterating over columns over range fixed   - reusing cell template is not updating index   - test data excels boolean cell type fixed 2. Additional small refactor
</commit_message>
<xml_diff>
--- a/src/test/resources/person-data.xlsx
+++ b/src/test/resources/person-data.xlsx
@@ -105,11 +105,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
-    <numFmt numFmtId="166" formatCode="HH:MM:SS"/>
-    <numFmt numFmtId="167" formatCode="YYYY\-MM\-DD\ HH:MM"/>
+    <numFmt numFmtId="165" formatCode="&quot;PRAWDA&quot;;&quot;PRAWDA&quot;;&quot;FAŁSZ&quot;"/>
+    <numFmt numFmtId="166" formatCode="YYYY\-MM\-DD"/>
+    <numFmt numFmtId="167" formatCode="HH:MM:SS"/>
+    <numFmt numFmtId="168" formatCode="YYYY\-MM\-DD\ HH:MM"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -179,7 +180,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -193,6 +194,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -216,7 +221,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J12" activeCellId="0" sqref="J12"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -260,17 +265,16 @@
       <c r="C2" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="0" t="n">
-        <f aca="false">IF(1,TRUE())</f>
-        <v>1</v>
-      </c>
-      <c r="E2" s="1" t="n">
+      <c r="D2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="n">
         <v>32874</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>1000</v>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="G2" s="3" t="n">
         <v>0.375</v>
       </c>
       <c r="H2" s="0" t="n">
@@ -287,17 +291,16 @@
       <c r="C3" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="0" t="n">
-        <f aca="false">IF(0,TRUE())</f>
+      <c r="D3" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="E3" s="2" t="n">
         <v>29221</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>2000</v>
       </c>
-      <c r="G3" s="2" t="n">
+      <c r="G3" s="3" t="n">
         <v>0.416666666666667</v>
       </c>
       <c r="H3" s="0" t="n">
@@ -314,17 +317,16 @@
       <c r="C4" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="0" t="n">
-        <f aca="false">IF(1,TRUE())</f>
-        <v>1</v>
-      </c>
-      <c r="E4" s="1" t="n">
+      <c r="D4" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2" t="n">
         <v>27395</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>5000</v>
       </c>
-      <c r="G4" s="2" t="n">
+      <c r="G4" s="3" t="n">
         <v>0.333333333333333</v>
       </c>
       <c r="H4" s="0" t="n">
@@ -341,17 +343,16 @@
       <c r="C5" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="0" t="n">
-        <f aca="false">IF(1,TRUE())</f>
-        <v>1</v>
-      </c>
-      <c r="E5" s="1" t="n">
+      <c r="D5" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2" t="n">
         <v>31048</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>10000</v>
       </c>
-      <c r="G5" s="2" t="n">
+      <c r="G5" s="3" t="n">
         <v>0.3125</v>
       </c>
       <c r="H5" s="0" t="n">
@@ -424,10 +425,10 @@
       <c r="D2" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="E2" s="2" t="n">
         <v>44196</v>
       </c>
-      <c r="F2" s="3" t="n">
+      <c r="F2" s="4" t="n">
         <v>40188.53125</v>
       </c>
     </row>
@@ -444,10 +445,10 @@
       <c r="D3" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="E3" s="2" t="n">
         <v>45657</v>
       </c>
-      <c r="F3" s="3" t="n">
+      <c r="F3" s="4" t="n">
         <v>40189.40625</v>
       </c>
     </row>
@@ -464,10 +465,10 @@
       <c r="D4" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="1" t="n">
+      <c r="E4" s="2" t="n">
         <v>47848</v>
       </c>
-      <c r="F4" s="3" t="n">
+      <c r="F4" s="4" t="n">
         <v>40190.7814236111</v>
       </c>
     </row>
@@ -484,10 +485,10 @@
       <c r="D5" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="1" t="n">
+      <c r="E5" s="2" t="n">
         <v>43830</v>
       </c>
-      <c r="F5" s="3" t="n">
+      <c r="F5" s="4" t="n">
         <v>40191.8333333333</v>
       </c>
     </row>

</xml_diff>